<commit_message>
update read me and client rates file
</commit_message>
<xml_diff>
--- a/Client Rates Folder/Current Client Rates - Client Minimum - Example Data.xlsx
+++ b/Client Rates Folder/Current Client Rates - Client Minimum - Example Data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericnaon/Desktop/Example invoicing program/Client Rates Folder/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericnaon/Desktop/Desktop - Eric’s MacBook Pro/Git/automatic_invoicing/Client Rates Folder/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{141D9A37-AC26-474C-8407-7C0A05E126F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F12EA356-B65C-C046-9DC7-4F8832FF7ABE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="760" yWindow="500" windowWidth="28040" windowHeight="16020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="295">
   <si>
     <t>Location</t>
   </si>
@@ -911,9 +911,6 @@
   </si>
   <si>
     <t>40.2</t>
-  </si>
-  <si>
-    <t>Senior Supervisor Rate</t>
   </si>
   <si>
     <t>29.45</t>
@@ -1776,8 +1773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A131" workbookViewId="0">
-      <selection activeCell="D147" sqref="D147"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1806,13 +1803,10 @@
       <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>293</v>
-      </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>201</v>
@@ -2138,7 +2132,7 @@
         <v>26</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E25" s="3">
         <f t="shared" si="0"/>
@@ -2386,9 +2380,6 @@
         <f t="shared" si="0"/>
         <v>34.659999999999997</v>
       </c>
-      <c r="F44" s="2" t="s">
-        <v>174</v>
-      </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
@@ -2473,9 +2464,6 @@
         <f t="shared" si="0"/>
         <v>39.5</v>
       </c>
-      <c r="F51" s="2" t="s">
-        <v>218</v>
-      </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
@@ -2649,7 +2637,7 @@
         <v>23.5</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>66</v>
       </c>
@@ -2661,7 +2649,7 @@
         <v>24.5</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>67</v>
       </c>
@@ -2673,7 +2661,7 @@
         <v>25.5</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>68</v>
       </c>
@@ -2685,7 +2673,7 @@
         <v>26.5</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>69</v>
       </c>
@@ -2697,7 +2685,7 @@
         <v>27.5</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>70</v>
       </c>
@@ -2709,7 +2697,7 @@
         <v>28.5</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>71</v>
       </c>
@@ -2721,7 +2709,7 @@
         <v>29.5</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>72</v>
       </c>
@@ -2733,7 +2721,7 @@
         <v>30.5</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>73</v>
       </c>
@@ -2745,7 +2733,7 @@
         <v>31.5</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>74</v>
       </c>
@@ -2760,7 +2748,7 @@
         <v>32.5</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>75</v>
       </c>
@@ -2772,7 +2760,7 @@
         <v>42.5</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>76</v>
       </c>
@@ -2787,7 +2775,7 @@
         <v>43.5</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>77</v>
       </c>
@@ -2802,7 +2790,7 @@
         <v>44.5</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>78</v>
       </c>
@@ -2814,7 +2802,7 @@
         <v>45.5</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>79</v>
       </c>
@@ -2826,7 +2814,7 @@
         <v>40.200000000000003</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>80</v>
       </c>
@@ -2838,7 +2826,7 @@
         <v>40.299999999999997</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>81</v>
       </c>
@@ -2848,9 +2836,6 @@
       <c r="E80" s="3">
         <f t="shared" si="1"/>
         <v>40.4</v>
-      </c>
-      <c r="F80" s="2" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.2">
@@ -3318,9 +3303,6 @@
         <f t="shared" si="1"/>
         <v>41.72</v>
       </c>
-      <c r="F116" s="2" t="s">
-        <v>175</v>
-      </c>
       <c r="J116" s="1"/>
     </row>
     <row r="117" spans="1:10" x14ac:dyDescent="0.2">
@@ -3676,9 +3658,6 @@
         <f t="shared" si="2"/>
         <v>42</v>
       </c>
-      <c r="F144" s="2" t="s">
-        <v>217</v>
-      </c>
     </row>
     <row r="145" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
@@ -3849,9 +3828,6 @@
       <c r="E157" s="3">
         <f t="shared" si="2"/>
         <v>33.64</v>
-      </c>
-      <c r="F157" s="2" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="158" spans="1:10" x14ac:dyDescent="0.2">

</xml_diff>